<commit_message>
add header deadline column
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR002.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR002.xlsx
@@ -224,7 +224,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -241,6 +241,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -543,7 +546,7 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="11.25"/>
@@ -560,37 +563,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
@@ -603,7 +606,7 @@
       <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="3">

</xml_diff>

<commit_message>
hot fix header template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR002.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR002.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\KDR002 Sua excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nws\Desktop\KDR002_SuaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -212,7 +212,9 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -546,7 +548,7 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="11.25"/>
@@ -660,19 +662,20 @@
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="J1:O1"/>
-    <mergeCell ref="P1:W1"/>
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:W1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader xml:space="preserve">&amp;L&amp;"ＭＳ ゴシック,標準"日通システム株式会社&amp;C&amp;"ＭＳ ゴシック,標準"&amp;16年休管理表
-&amp;R&amp;"ＭＳ ゴシック,標準"yyyy/mm/dd HH:MM　
+    <oddHeader xml:space="preserve">&amp;L&amp;"ＭＳ ゴシック,Regular"日通システム株式会社&amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16年休管理表
+&amp;R&amp;"ＭＳ ゴシック,Regular"yyyy/mm/dd HH:MM　
 page&amp;P&amp;Y
 &amp;Y
 </oddHeader>

</xml_diff>

<commit_message>
Fix bug KDR002 #119257, #119258, #119259
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR002.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR002.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\UniversalK_clone\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABC037B-381D-4422-97D0-E8D8D7D69235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1938B35A-2B0C-455E-84AF-BD374D0906A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="改ページなし" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
     <rPh sb="0" eb="2">
       <t>シャイン</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>付与日</t>
@@ -65,7 +65,7 @@
     <rPh sb="2" eb="3">
       <t>ビ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>付与数</t>
@@ -75,14 +75,14 @@
     <rPh sb="2" eb="3">
       <t>スウ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>残数</t>
     <rPh sb="0" eb="2">
       <t>ザンスウ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>次回付与日</t>
@@ -95,7 +95,7 @@
     <rPh sb="4" eb="5">
       <t>ビ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>使用数</t>
@@ -105,7 +105,7 @@
     <rPh sb="2" eb="3">
       <t>スウ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>&amp;=I18N.KDR002_11(bean)</t>
@@ -118,18 +118,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Meiryo UI"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="源ノ角ゴシック Normal"/>
       <family val="2"/>
       <charset val="128"/>
     </font>
@@ -240,39 +233,33 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,122 +549,162 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="3.109375" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="6.140625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="5.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" style="1" customWidth="1"/>
-    <col min="9" max="22" width="5.28515625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9.28515625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="3.140625" style="1"/>
+    <col min="1" max="1" width="8.109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="8" customWidth="1"/>
+    <col min="3" max="4" width="6.109375" style="8" customWidth="1"/>
+    <col min="5" max="7" width="5.33203125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" style="8" customWidth="1"/>
+    <col min="9" max="22" width="5.33203125" style="8" customWidth="1"/>
+    <col min="23" max="23" width="9.33203125" style="8" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="3.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:23" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
     </row>
-    <row r="2" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:23" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="3">
         <v>1</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="1">
         <v>2</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="1">
         <v>3</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="1">
         <v>4</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="1">
         <v>5</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="1">
         <v>6</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="1">
         <v>7</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="1">
         <v>8</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="1">
         <v>9</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="1">
         <v>10</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="1">
         <v>11</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="1">
         <v>12</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="1">
         <v>13</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2" s="1">
         <v>14</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="1">
         <v>15</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15" customHeight="1"/>
+    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:B2"/>
@@ -686,7 +713,7 @@
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:W1"/>
   </mergeCells>
-  <phoneticPr fontId="2"/>
+  <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>